<commit_message>
Delete i¡old version inputIncidencias.xlsx in Examples
</commit_message>
<xml_diff>
--- a/examples/traffic/input/InputIncidencias.xlsx
+++ b/examples/traffic/input/InputIncidencias.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ednaruckhaus/Documents/GitHub/Mapeathor/examples/traffic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B826E0-952E-FA4D-90C2-F9DEDABE227C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6797B1BA-AF57-B84C-A8EB-38D0D5FA22FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="500" windowWidth="30440" windowHeight="19740" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="PredicateObjectMaps" sheetId="4" r:id="rId4"/>
     <sheet name="Functions" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="91">
   <si>
     <t>Prefix</t>
   </si>
@@ -285,9 +285,6 @@
     <t>estraf:incidenciaEnTramo</t>
   </si>
   <si>
-    <t>recurso-trafico:punto/t-{id_incidencia_nuevo}</t>
-  </si>
-  <si>
     <t>dct:description</t>
   </si>
   <si>
@@ -307,6 +304,12 @@
   </si>
   <si>
     <t>http://vocab.ciudadesabiertas.es/recurso/transporte/trafico/tramo/t-{id_incidencia_nuevo}</t>
+  </si>
+  <si>
+    <t>iri</t>
+  </si>
+  <si>
+    <t>recurso-trafico:tramot-{id_incidencia_nuevo}</t>
   </si>
 </sst>
 </file>
@@ -808,7 +811,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>72</v>
@@ -986,7 +989,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -994,10 +997,10 @@
         <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1011,7 +1014,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1150,7 +1153,7 @@
         <v>73</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
         <v>31</v>
@@ -1170,7 +1173,7 @@
         <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="G9" t="s">
         <v>53</v>
@@ -1181,10 +1184,10 @@
         <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="G10" t="s">
         <v>53</v>
@@ -1237,7 +1240,7 @@
         <v>78</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
@@ -1248,10 +1251,10 @@
     </row>
     <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>

</xml_diff>